<commit_message>
Get country and region rebate
</commit_message>
<xml_diff>
--- a/app/data/EV_list_France.xlsx
+++ b/app/data/EV_list_France.xlsx
@@ -1292,11 +1292,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11439,7 +11439,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11469,12 +11469,12 @@
         <v>126</v>
       </c>
       <c r="B2" s="76" t="n">
-        <v>12345</v>
-      </c>
-      <c r="C2" s="76" t="s">
+        <v>111111</v>
+      </c>
+      <c r="C2" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="76" t="s">
         <v>127</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New code to get tax and utility
</commit_message>
<xml_diff>
--- a/app/data/EV_list_France.xlsx
+++ b/app/data/EV_list_France.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cars" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,6 @@
     <sheet name="Gas" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Electricity" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Fees" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Sources" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="141">
   <si>
     <t xml:space="preserve">Make</t>
   </si>
@@ -421,48 +420,6 @@
     <t xml:space="preserve">Rate</t>
   </si>
   <si>
-    <t xml:space="preserve">Federal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alberta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">British Columbia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manitoba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Brunswick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Newfoundland and Labrador</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northwest Territories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nova Scotia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nunavut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ontario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prince Edward Island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quebec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saskatchewan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yukon</t>
-  </si>
-  <si>
     <t xml:space="preserve">Source: canadadrives.ca</t>
   </si>
   <si>
@@ -491,39 +448,6 @@
   </si>
   <si>
     <t xml:space="preserve">Amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rebates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plugndrive.ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.plugndrive.ca/electric-vehicle-incentives/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">canadadrives.ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Statistics Canada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electricity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">energyhub.com</t>
   </si>
 </sst>
 </file>
@@ -537,7 +461,7 @@
     <numFmt numFmtId="167" formatCode="0.00%"/>
     <numFmt numFmtId="168" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -622,13 +546,6 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -987,7 +904,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="86">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1332,14 +1249,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="46" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1732,7 +1641,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
@@ -1757,7 +1666,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
@@ -1784,7 +1693,7 @@
       <c r="J4" s="11"/>
       <c r="K4" s="18"/>
     </row>
-    <row r="5" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
@@ -1811,7 +1720,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
@@ -1845,7 +1754,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
@@ -1874,7 +1783,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
         <v>35</v>
       </c>
@@ -1907,7 +1816,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
         <v>21</v>
       </c>
@@ -1932,7 +1841,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="18"/>
     </row>
-    <row r="10" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
         <v>42</v>
       </c>
@@ -1965,7 +1874,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
         <v>28</v>
       </c>
@@ -2000,7 +1909,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
         <v>25</v>
       </c>
@@ -2031,7 +1940,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
         <v>51</v>
       </c>
@@ -2066,7 +1975,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
         <v>25</v>
       </c>
@@ -2099,7 +2008,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
         <v>35</v>
       </c>
@@ -2134,7 +2043,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
         <v>11</v>
       </c>
@@ -2167,7 +2076,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="17" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
@@ -2201,7 +2110,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="18" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
         <v>28</v>
       </c>
@@ -2236,7 +2145,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="s">
         <v>63</v>
       </c>
@@ -2259,7 +2168,7 @@
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
         <v>21</v>
       </c>
@@ -2288,7 +2197,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="21" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
         <v>17</v>
       </c>
@@ -2321,7 +2230,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
         <v>35</v>
       </c>
@@ -2356,7 +2265,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="23" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
         <v>11</v>
       </c>
@@ -2391,7 +2300,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="24" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
         <v>51</v>
       </c>
@@ -2424,7 +2333,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="25" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
         <v>21</v>
       </c>
@@ -2453,7 +2362,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="26" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="s">
         <v>11</v>
       </c>
@@ -2486,7 +2395,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="27" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
         <v>28</v>
       </c>
@@ -2520,7 +2429,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="28" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
         <v>17</v>
       </c>
@@ -2555,7 +2464,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="29" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
         <v>25</v>
       </c>
@@ -2588,7 +2497,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="30" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
         <v>11</v>
       </c>
@@ -2623,7 +2532,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="31" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="12" t="s">
         <v>28</v>
       </c>
@@ -2654,7 +2563,7 @@
       </c>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="s">
         <v>84</v>
       </c>
@@ -2687,7 +2596,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="33" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="s">
         <v>25</v>
       </c>
@@ -2720,7 +2629,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="34" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="s">
         <v>11</v>
       </c>
@@ -2755,7 +2664,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="35" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="12" t="s">
         <v>11</v>
       </c>
@@ -11438,7 +11347,7 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -11524,124 +11433,33 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="80" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="81" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="81" t="n">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="80" t="s">
+      <c r="B3" s="82" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="81" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="80" t="s">
-        <v>133</v>
-      </c>
-      <c r="B4" s="81" t="n">
-        <v>0.07</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="80" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" s="81" t="n">
-        <v>0.07</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="80" t="s">
-        <v>135</v>
-      </c>
-      <c r="B6" s="81" t="n">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="80" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" s="81" t="n">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="80" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" s="81" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="80" t="s">
-        <v>138</v>
-      </c>
-      <c r="B9" s="81" t="n">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="80" t="s">
-        <v>139</v>
-      </c>
-      <c r="B10" s="81" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="80" t="s">
-        <v>140</v>
-      </c>
-      <c r="B11" s="81" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="80" t="s">
-        <v>141</v>
-      </c>
-      <c r="B12" s="81" t="n">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="80" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="81" t="n">
-        <v>0.09975</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="80" t="s">
-        <v>143</v>
-      </c>
-      <c r="B14" s="81" t="n">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="80" t="s">
-        <v>144</v>
-      </c>
-      <c r="B15" s="81" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="82" t="s">
-        <v>145</v>
-      </c>
-      <c r="B16" s="82" t="s">
-        <v>146</v>
-      </c>
-    </row>
+    </row>
+    <row r="4" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -11656,7 +11474,7 @@
     <row r="28" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -11666,19 +11484,19 @@
     <row r="38" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -11698,10 +11516,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11714,119 +11532,23 @@
         <v>122</v>
       </c>
       <c r="B1" s="83" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="75" t="s">
-        <v>132</v>
+      <c r="A2" s="80" t="s">
+        <v>126</v>
       </c>
       <c r="B2" s="75" t="n">
         <v>146</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="75" t="s">
-        <v>133</v>
-      </c>
-      <c r="B3" s="75" t="n">
-        <v>187.8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="75" t="s">
+      <c r="A3" s="82" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="75" t="n">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="75" t="s">
+      <c r="B3" s="82" t="s">
         <v>135</v>
-      </c>
-      <c r="B5" s="75" t="n">
-        <v>159.1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="75" t="s">
-        <v>136</v>
-      </c>
-      <c r="B6" s="75" t="n">
-        <v>165.5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="75" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="75" t="n">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="75" t="s">
-        <v>138</v>
-      </c>
-      <c r="B8" s="75" t="n">
-        <v>151.4</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="75" t="s">
-        <v>139</v>
-      </c>
-      <c r="B9" s="75" t="n">
-        <v>158.8</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="75" t="s">
-        <v>140</v>
-      </c>
-      <c r="B10" s="75" t="n">
-        <v>156.1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="75" t="s">
-        <v>141</v>
-      </c>
-      <c r="B11" s="75" t="n">
-        <v>161.2</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="75" t="s">
-        <v>142</v>
-      </c>
-      <c r="B12" s="75" t="n">
-        <v>166.4</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="75" t="s">
-        <v>143</v>
-      </c>
-      <c r="B13" s="75" t="n">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="75" t="s">
-        <v>144</v>
-      </c>
-      <c r="B14" s="75" t="n">
-        <v>183.9</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="82" t="s">
-        <v>148</v>
-      </c>
-      <c r="B15" s="82" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -11845,10 +11567,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11861,119 +11583,23 @@
         <v>122</v>
       </c>
       <c r="B1" s="79" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="80" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B2" s="80" t="n">
         <v>16.6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="80" t="s">
-        <v>133</v>
-      </c>
-      <c r="B3" s="80" t="n">
-        <v>12.6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="80" t="s">
-        <v>134</v>
-      </c>
-      <c r="B4" s="80" t="n">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="80" t="s">
-        <v>135</v>
-      </c>
-      <c r="B5" s="80" t="n">
-        <v>12.7</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="80" t="s">
-        <v>136</v>
-      </c>
-      <c r="B6" s="80" t="n">
-        <v>13.8</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="80" t="s">
+      <c r="A3" s="82" t="s">
         <v>137</v>
       </c>
-      <c r="B7" s="80" t="n">
-        <v>38.2</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="80" t="s">
+      <c r="B3" s="82" t="s">
         <v>138</v>
-      </c>
-      <c r="B8" s="80" t="n">
-        <v>17.1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="80" t="s">
-        <v>139</v>
-      </c>
-      <c r="B9" s="80" t="n">
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="80" t="s">
-        <v>140</v>
-      </c>
-      <c r="B10" s="80" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="80" t="s">
-        <v>141</v>
-      </c>
-      <c r="B11" s="80" t="n">
-        <v>17.4</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="80" t="s">
-        <v>142</v>
-      </c>
-      <c r="B12" s="80" t="n">
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="80" t="s">
-        <v>143</v>
-      </c>
-      <c r="B13" s="80" t="n">
-        <v>18.1</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="80" t="s">
-        <v>144</v>
-      </c>
-      <c r="B14" s="80" t="n">
-        <v>18.7</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="82" t="s">
-        <v>151</v>
-      </c>
-      <c r="B15" s="82" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -11994,8 +11620,8 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D62" activeCellId="0" sqref="D62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12005,10 +11631,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="84" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B1" s="84" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12132,91 +11758,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="50.49"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="86" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="86" t="s">
-        <v>156</v>
-      </c>
-      <c r="C1" s="86" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="82" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="82" t="s">
-        <v>158</v>
-      </c>
-      <c r="C2" s="87" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="82" t="s">
-        <v>160</v>
-      </c>
-      <c r="B3" s="82" t="s">
-        <v>161</v>
-      </c>
-      <c r="C3" s="82" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="82" t="s">
-        <v>162</v>
-      </c>
-      <c r="B4" s="82" t="s">
-        <v>163</v>
-      </c>
-      <c r="C4" s="82" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="82" t="s">
-        <v>164</v>
-      </c>
-      <c r="B5" s="82" t="s">
-        <v>165</v>
-      </c>
-      <c r="C5" s="82" t="s">
-        <v>152</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://www.plugndrive.ca/electric-vehicle-incentives/"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed calculation of rebates
</commit_message>
<xml_diff>
--- a/app/data/EV_list_France.xlsx
+++ b/app/data/EV_list_France.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cars" sheetId="1" state="visible" r:id="rId2"/>
@@ -1560,7 +1560,7 @@
   <dimension ref="A1:K1027"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11347,8 +11347,8 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I56" activeCellId="0" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11378,7 +11378,7 @@
         <v>126</v>
       </c>
       <c r="B2" s="76" t="n">
-        <v>111111</v>
+        <v>1000</v>
       </c>
       <c r="C2" s="77" t="s">
         <v>127</v>
@@ -11620,7 +11620,7 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
     </sheetView>
   </sheetViews>

</xml_diff>